<commit_message>
diagram relac con carrito de compras 13/12
</commit_message>
<xml_diff>
--- a/Tablas Relacionales (2).xlsx
+++ b/Tablas Relacionales (2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://siemens-my.sharepoint.com/personal/andres_richardson_siemens_com/Documents/Desktop/GRUPO_12_TRABAJO_INTEGRADOR/Grupo_12_Completar_Nombre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC5F24AE-7184-4DD7-B969-80B3B7DD2822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{BC5F24AE-7184-4DD7-B969-80B3B7DD2822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE2C4BB3-C203-4C6E-8C56-F3760A683F45}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="54">
   <si>
     <t>Users</t>
   </si>
@@ -126,9 +126,6 @@
     <t>quotesQuantity</t>
   </si>
   <si>
-    <t>updateData</t>
-  </si>
-  <si>
     <t>productsImages</t>
   </si>
   <si>
@@ -160,6 +157,33 @@
   </si>
   <si>
     <t>enum</t>
+  </si>
+  <si>
+    <t>Carts</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>qtyitems</t>
+  </si>
+  <si>
+    <t>deleteDate</t>
+  </si>
+  <si>
+    <t>sold</t>
+  </si>
+  <si>
+    <t>updateDate</t>
+  </si>
+  <si>
+    <t>updatedAt</t>
+  </si>
+  <si>
+    <t>createdAt</t>
+  </si>
+  <si>
+    <t>deletedAt</t>
   </si>
 </sst>
 </file>
@@ -213,7 +237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -432,11 +456,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -449,7 +512,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -464,34 +552,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1838,6 +1915,618 @@
         <a:xfrm flipH="1">
           <a:off x="8441765" y="5707529"/>
           <a:ext cx="171825" cy="119533"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>37353</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>92691</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>627529</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>104588</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="58 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B31DCA0-58CC-4142-BD73-E15DCEEAC6D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12886765" y="481162"/>
+          <a:ext cx="590176" cy="11897"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>620059</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>119529</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>627577</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>37356</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="29 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2DEFFF5-5A1A-4CDA-8AB6-E1FAE9F9B3C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13469471" y="508000"/>
+          <a:ext cx="7518" cy="485591"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>605119</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>59765</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>739588</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>70973</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="31 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D123BE45-997D-4E25-B1FE-55172B6B596D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13454531" y="1016000"/>
+          <a:ext cx="134469" cy="11208"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>612588</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>97118</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>732117</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="31 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{055D8572-16B4-4946-8048-221DD713EF54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="13462000" y="1053353"/>
+          <a:ext cx="119529" cy="29882"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>7471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>724647</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>52294</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="31 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE6CBBA0-F56F-444F-BC66-0DBFEE2F7E74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13484412" y="963706"/>
+          <a:ext cx="89647" cy="44823"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>144930</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>58327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>735106</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>70224</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="58 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33518AE9-CECE-4B78-924A-37AAFE8FD254}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12994342" y="820327"/>
+          <a:ext cx="590176" cy="11897"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>174860</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>179294</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>82177</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="29 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3479C040-E8CC-4B90-9BFA-3AE32F6B1C8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13024272" y="787400"/>
+          <a:ext cx="4434" cy="1394012"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>74706</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>123956</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>216647</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="58 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F28F084-3883-4F59-8B7C-7A0B4E9222A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4542118" y="2223191"/>
+          <a:ext cx="8523941" cy="10515"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>20966</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>80683</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>52294</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>141941</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="29 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{351AB323-CD89-4423-BF8D-41CAD4E8BF1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4488378" y="1036918"/>
+          <a:ext cx="31328" cy="1204258"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>29882</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>7472</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>93382</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="31 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F96B23E5-EA1F-4A71-84B1-48A87D1229E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2973294" y="941294"/>
+          <a:ext cx="1501590" cy="108323"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>627529</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>141941</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="31 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{294BD57E-ECEF-4B09-BAF0-803E69702C32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13476941" y="717176"/>
+          <a:ext cx="134471" cy="67236"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>612588</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>82176</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>739588</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>119529</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="31 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41395639-2D84-4705-82E3-203713141D1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="13462000" y="844176"/>
+          <a:ext cx="127000" cy="37353"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2187,8 +2876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:N10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2199,278 +2888,356 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="13" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="20"/>
-      <c r="O2" s="21" t="s">
+      <c r="N2" s="19"/>
+      <c r="O2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" s="26"/>
+      <c r="S2" s="27" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="19" t="s">
+      <c r="G3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="20"/>
-      <c r="K3" s="21" t="s">
+      <c r="J3" s="19"/>
+      <c r="K3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="15" t="s">
-        <v>41</v>
+      <c r="O3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" s="30" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="14"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="14" t="s">
+      <c r="G4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" s="14"/>
+      <c r="K4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="9"/>
       <c r="N4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="15" t="s">
-        <v>44</v>
+      <c r="O4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="16" t="s">
+      <c r="C5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="17" t="s">
+      <c r="G5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" s="14"/>
+      <c r="K5" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="9"/>
       <c r="N5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="15" t="s">
-        <v>43</v>
+      <c r="O5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="14"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="M6" s="14"/>
+      <c r="C6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="9"/>
       <c r="N6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="15" t="s">
-        <v>43</v>
+      <c r="O6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="14"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" s="14"/>
+      <c r="C7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="9"/>
       <c r="N7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O7" s="15" t="s">
-        <v>43</v>
+      <c r="O7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="14"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="20"/>
-      <c r="J8" s="21" t="s">
+      <c r="C8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="M8" s="14"/>
+      <c r="M8" s="9"/>
       <c r="N8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O8" s="15" t="s">
+      <c r="O8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S8" s="10" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="14" t="s">
+      <c r="C9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>5</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J9" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="M9" s="14"/>
+      <c r="J9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="9"/>
       <c r="N9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O9" s="15" t="s">
-        <v>43</v>
+      <c r="O9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S9" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="14"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="14"/>
+      <c r="C10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="I10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="M10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="N10" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" s="11"/>
+      <c r="N10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="O10" s="23" t="s">
-        <v>45</v>
+      <c r="O10" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="S10" s="13" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="14"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="17" t="s">
+      <c r="C11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="18" t="s">
-        <v>43</v>
+      <c r="J11" s="13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="14"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>41</v>
+      <c r="C12" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>44</v>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="9"/>
+      <c r="B13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="9"/>
+      <c r="B14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="21" t="s">
+      <c r="I16" s="19"/>
+      <c r="J16" s="14" t="s">
         <v>26</v>
       </c>
       <c r="O16" t="s">
@@ -2480,24 +3247,24 @@
         <v>6</v>
       </c>
       <c r="Q16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="8:19" x14ac:dyDescent="0.35">
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="9" t="s">
         <v>5</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J17" s="15" t="s">
-        <v>41</v>
+      <c r="J17" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="O17" s="5">
         <v>1</v>
@@ -2516,12 +3283,14 @@
       </c>
     </row>
     <row r="18" spans="8:19" x14ac:dyDescent="0.35">
-      <c r="H18" s="14"/>
+      <c r="H18" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="I18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>41</v>
+        <v>36</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="O18" s="5">
         <v>2</v>
@@ -2540,12 +3309,12 @@
       </c>
     </row>
     <row r="19" spans="8:19" x14ac:dyDescent="0.35">
-      <c r="H19" s="14"/>
+      <c r="H19" s="9"/>
       <c r="I19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J19" s="22" t="s">
-        <v>41</v>
+      <c r="J19" s="15" t="s">
+        <v>40</v>
       </c>
       <c r="O19" s="5">
         <v>3</v>
@@ -2564,12 +3333,12 @@
       </c>
     </row>
     <row r="20" spans="8:19" x14ac:dyDescent="0.35">
-      <c r="H20" s="14"/>
+      <c r="H20" s="9"/>
       <c r="I20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J20" s="22" t="s">
-        <v>41</v>
+      <c r="J20" s="15" t="s">
+        <v>40</v>
       </c>
       <c r="O20" s="5">
         <v>4</v>
@@ -2582,12 +3351,12 @@
       </c>
     </row>
     <row r="21" spans="8:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H21" s="16"/>
-      <c r="I21" s="17" t="s">
+      <c r="H21" s="11"/>
+      <c r="I21" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J21" s="23" t="s">
-        <v>41</v>
+      <c r="J21" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="O21" s="5"/>
       <c r="P21" s="5">
@@ -2609,95 +3378,96 @@
       </c>
     </row>
     <row r="23" spans="8:19" x14ac:dyDescent="0.35">
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="21" t="s">
+      <c r="I23" s="19"/>
+      <c r="J23" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" spans="8:19" x14ac:dyDescent="0.35">
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="9" t="s">
         <v>5</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J24" s="15" t="s">
-        <v>41</v>
+      <c r="J24" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="8:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H25" s="16"/>
-      <c r="I25" s="17" t="s">
+      <c r="H25" s="11"/>
+      <c r="I25" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="J25" s="18" t="s">
-        <v>43</v>
+      <c r="J25" s="13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="8:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="27" spans="8:19" x14ac:dyDescent="0.35">
-      <c r="H27" s="19" t="s">
+      <c r="H27" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="21" t="s">
+      <c r="I27" s="19"/>
+      <c r="J27" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="8:19" x14ac:dyDescent="0.35">
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="9" t="s">
         <v>5</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J28" s="15" t="s">
-        <v>41</v>
+      <c r="J28" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="8:19" x14ac:dyDescent="0.35">
-      <c r="H29" s="14"/>
+      <c r="H29" s="9"/>
       <c r="I29" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J29" s="15" t="s">
-        <v>43</v>
+      <c r="J29" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="8:19" x14ac:dyDescent="0.35">
-      <c r="H30" s="14"/>
+      <c r="H30" s="9"/>
       <c r="I30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J30" s="22" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="J30" s="15" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="8:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H31" s="16" t="s">
+      <c r="H31" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I31" s="24" t="s">
+      <c r="I31" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J31" s="16" t="s">
         <v>40</v>
-      </c>
-      <c r="J31" s="23" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="Q2:R2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>